<commit_message>
changed dpi became 96
</commit_message>
<xml_diff>
--- a/xlsxwriter/test/comparison/xlsx_files/image_wmf_1.xlsx
+++ b/xlsxwriter/test/comparison/xlsx_files/image_wmf_1.xlsx
@@ -61,18 +61,18 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1026" name="Picture 2" descr="example_1"/>
+        <xdr:cNvPr id="1025" name="Picture 2" descr="example_1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -86,13 +86,19 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2438400" y="1524000"/>
+          <a:off x="2438400" y="1409700"/>
           <a:ext cx="504825" cy="466725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -112,7 +118,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1027" name="Picture 3" descr="example_2"/>
+        <xdr:cNvPr id="1026" name="Picture 3" descr="example_2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -133,6 +139,12 @@
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -152,7 +164,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1028" name="Picture 4" descr="Python"/>
+        <xdr:cNvPr id="1027" name="Picture 4" descr="Python"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -173,6 +185,12 @@
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -467,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>